<commit_message>
online UG model results stats update
</commit_message>
<xml_diff>
--- a/lme_results/ug_T1/ug_envy.xlsx
+++ b/lme_results/ug_T1/ug_envy.xlsx
@@ -392,16 +392,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>6.29404897494841</v>
+        <v>2.7668667708129</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0685807678479692</v>
+        <v>0.154719166873387</v>
       </c>
       <c r="D2" t="n">
-        <v>91.7757145691507</v>
+        <v>17.8831545355795</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000255561736657851</v>
+        <v>0.00000000000000000000000000000000000000000198838086898623</v>
       </c>
     </row>
     <row r="3">
@@ -409,16 +409,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>0.355132598562625</v>
+        <v>0.130824900782017</v>
       </c>
       <c r="C3" t="n">
-        <v>0.138692791261486</v>
+        <v>0.313412707356774</v>
       </c>
       <c r="D3" t="n">
-        <v>2.56056998588392</v>
+        <v>0.417420537556865</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0113930487043003</v>
+        <v>0.676847136867132</v>
       </c>
     </row>
     <row r="4">
@@ -426,16 +426,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.121519459210214</v>
+        <v>0.0235433211371859</v>
       </c>
       <c r="C4" t="n">
-        <v>0.137227503693331</v>
+        <v>0.309449197675248</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.885532826435283</v>
+        <v>0.0760813772149233</v>
       </c>
       <c r="E4" t="n">
-        <v>0.37722360043912</v>
+        <v>0.939435257857624</v>
       </c>
     </row>
     <row r="5">
@@ -443,16 +443,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.247837070717715</v>
+        <v>-0.0432914555763041</v>
       </c>
       <c r="C5" t="n">
-        <v>0.277944985317329</v>
+        <v>0.62561652674361</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.891676712334853</v>
+        <v>-0.069198068985869</v>
       </c>
       <c r="E5" t="n">
-        <v>0.373930777273154</v>
+        <v>0.944905506194815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>